<commit_message>
Supermarket Checkout test run commit
</commit_message>
<xml_diff>
--- a/Python Examples/Assessment2_SimonJohnson/chart1.xlsx
+++ b/Python Examples/Assessment2_SimonJohnson/chart1.xlsx
@@ -598,7 +598,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
@@ -618,7 +618,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>